<commit_message>
Cambio Orden de compra
</commit_message>
<xml_diff>
--- a/docs/historias-de-usuarios.xlsx
+++ b/docs/historias-de-usuarios.xlsx
@@ -1,30 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
-  <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\low\Documents\GitHub\upb-motors\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\USUARIO\Documents\GitHub\upb-motors\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{216C0482-5939-4460-AD0C-D0A5B48166CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
     <sheet name="Todos" sheetId="6" r:id="rId2"/>
     <sheet name="Despacho" sheetId="2" r:id="rId3"/>
-    <sheet name="Recursos humanos" sheetId="3" r:id="rId4"/>
-    <sheet name="Inventario" sheetId="5" r:id="rId5"/>
-    <sheet name="Vendedor" sheetId="7" r:id="rId6"/>
+    <sheet name="Inventario" sheetId="5" r:id="rId4"/>
+    <sheet name="Vendedor" sheetId="7" r:id="rId5"/>
+    <sheet name="Recursos humanos" sheetId="3" r:id="rId6"/>
     <sheet name="Gerente" sheetId="8" r:id="rId7"/>
     <sheet name="Taller" sheetId="10" r:id="rId8"/>
     <sheet name="Concesionario" sheetId="11" r:id="rId9"/>
     <sheet name="Consorcio " sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="161">
   <si>
     <t>Usuarios</t>
   </si>
@@ -93,27 +92,12 @@
     <t>D3</t>
   </si>
   <si>
-    <t>Buscar ordenes de compra pendientes</t>
-  </si>
-  <si>
     <t>D4</t>
   </si>
   <si>
     <t>Ver orden de compra</t>
   </si>
   <si>
-    <t>D5</t>
-  </si>
-  <si>
-    <t>Avanzar orden de compra</t>
-  </si>
-  <si>
-    <t>D6</t>
-  </si>
-  <si>
-    <t>Retroceder orden de compra</t>
-  </si>
-  <si>
     <t>Nombre del producto</t>
   </si>
   <si>
@@ -138,9 +122,6 @@
     <t>Caracteristicas de la orden de compra</t>
   </si>
   <si>
-    <t>La orden de compra cambia de estado</t>
-  </si>
-  <si>
     <t>Notas</t>
   </si>
   <si>
@@ -538,12 +519,15 @@
   </si>
   <si>
     <t>Cualquier empresa del consorcio puede listar productos en mi inventario para cerrar  tratos con nosotros</t>
+  </si>
+  <si>
+    <t>Buscar ordenes de compra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -978,33 +962,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E1058C6-D65F-FA4B-8FB7-73633D0CA677}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F9" sqref="B4:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="1"/>
       <c r="E2" s="16" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F2" s="16"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1019,35 +1003,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1055,13 +1039,13 @@
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
@@ -1069,20 +1053,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="120" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1095,16 +1079,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A413B8-F2B8-354D-8395-24F677DA194D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>8</v>
       </c>
@@ -1118,24 +1102,24 @@
         <v>13</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="201.6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="225" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1144,16 +1128,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C10F524-DA89-6742-AC85-4D6CAF2A9E58}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
@@ -1167,60 +1151,60 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="105" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E5" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1229,21 +1213,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C1B93A-92A9-6C47-931E-68161C0C4246}">
-  <dimension ref="B2:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F12"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1257,10 +1241,10 @@
         <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1268,14 +1252,14 @@
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1283,233 +1267,220 @@
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="2:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+    </row>
+    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="2:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D10" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-    </row>
-    <row r="11" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="B13" s="2">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B14" s="2">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2F40E5-6CBA-D84C-95FF-05B780D8EA36}">
-  <dimension ref="B2:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="2:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="2:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="2:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="2:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="3"/>
+      <c r="F2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1517,16 +1488,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72753584-440B-B240-98A4-3A428D54E3EA}">
-  <dimension ref="B2:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:F9"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1540,98 +1511,158 @@
         <v>13</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>86</v>
+        <v>136</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>89</v>
+        <v>137</v>
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>90</v>
+        <v>138</v>
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>94</v>
+        <v>140</v>
       </c>
       <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1639,181 +1670,104 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677488BD-6B46-5E48-9F20-9F5A315FF365}">
-  <dimension ref="B2:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="2:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="2:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="F12" s="4"/>
+      <c r="F2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="2:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="2:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="2:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="2:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1821,16 +1775,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D71B92-910E-1D45-91CE-FE5D6E8F4A26}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
@@ -1844,32 +1798,32 @@
         <v>13</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="2:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F4" s="4"/>
     </row>
@@ -1879,16 +1833,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E618B4E-B304-5D4F-A6B1-8EA548E8D529}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>8</v>
       </c>
@@ -1902,21 +1856,21 @@
         <v>13</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="216" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="225" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F3" s="13"/>
     </row>
@@ -1926,16 +1880,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18ED5395-63FA-EC4D-AFCA-CBAAE0EF9364}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
         <v>8</v>
       </c>
@@ -1949,21 +1903,21 @@
         <v>13</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F3" s="14"/>
     </row>

</xml_diff>